<commit_message>
Bugfix to my last Bugfix
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\MSEProj01\ExcelDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MSEProj01\ExcelDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,15 +68,6 @@
     <t>Started New</t>
   </si>
   <si>
-    <t>02c54b4d-e85b-4bdf-8bb6-57d07f872f1c</t>
-  </si>
-  <si>
-    <t>Save My Job Project</t>
-  </si>
-  <si>
-    <t>Server Jimmy</t>
-  </si>
-  <si>
     <t>Website Creation</t>
   </si>
   <si>
@@ -84,6 +75,15 @@
   </si>
   <si>
     <t>P.O.C</t>
+  </si>
+  <si>
+    <t>02c54b4d-e85b-4bdf-8bb6-48d07f872f1c</t>
+  </si>
+  <si>
+    <t>Project Love</t>
+  </si>
+  <si>
+    <t>Chez Martha</t>
   </si>
 </sst>
 </file>
@@ -214,6 +214,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -249,6 +266,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,22 +438,22 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,12 +479,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -462,21 +496,21 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -488,21 +522,21 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -514,21 +548,21 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -540,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Adds security check to Email Adapter
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MSEProj01\ExcelDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Jones\Source\Repos\MSEProj01\ExcelDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>ProjectID</t>
   </si>
@@ -56,34 +56,31 @@
     <t>Done</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Started</t>
-  </si>
-  <si>
-    <t>Trello Board</t>
-  </si>
-  <si>
-    <t>Started New</t>
-  </si>
-  <si>
-    <t>Website Creation</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>P.O.C</t>
-  </si>
-  <si>
     <t>02c54b4d-e85b-4bdf-8bb6-48d07f872f1c</t>
   </si>
   <si>
-    <t>Project Love</t>
-  </si>
-  <si>
-    <t>Chez Martha</t>
+    <t>Excel Security</t>
+  </si>
+  <si>
+    <t>Laura's Test Environment</t>
+  </si>
+  <si>
+    <t>Working Environment</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>April 10 2016</t>
+  </si>
+  <si>
+    <t>Test Number</t>
+  </si>
+  <si>
+    <t>Test Iteration</t>
+  </si>
+  <si>
+    <t>2B</t>
   </si>
 </sst>
 </file>
@@ -438,22 +435,22 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,12 +476,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -496,21 +493,21 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -522,21 +519,21 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -548,21 +545,21 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -574,13 +571,13 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ExcelDemo, Excel file, repaired Update method in ProjectUpdateController
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Jones\Source\Repos\MSEProj01\ExcelDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\MSEProj01\ExcelDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
-  <si>
-    <t>ProjectID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>ProjectName</t>
   </si>
@@ -38,49 +35,76 @@
     <t>VerticalID</t>
   </si>
   <si>
-    <t>Key1</t>
-  </si>
-  <si>
-    <t>Value1</t>
-  </si>
-  <si>
-    <t>Key2</t>
-  </si>
-  <si>
-    <t>Value2</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>02c54b4d-e85b-4bdf-8bb6-48d07f872f1c</t>
-  </si>
-  <si>
     <t>Excel Security</t>
   </si>
   <si>
     <t>Laura's Test Environment</t>
   </si>
   <si>
-    <t>Working Environment</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>April 10 2016</t>
-  </si>
-  <si>
-    <t>Test Number</t>
-  </si>
-  <si>
-    <t>Test Iteration</t>
-  </si>
-  <si>
-    <t>2B</t>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Laura's Build Environment</t>
+  </si>
+  <si>
+    <t>BR549</t>
+  </si>
+  <si>
+    <t>Target Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager </t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Add detail page</t>
+  </si>
+  <si>
+    <t>Convert to UpdatePackage</t>
+  </si>
+  <si>
+    <t>Update Contact page</t>
+  </si>
+  <si>
+    <t>Test Register function</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Bocephus</t>
+  </si>
+  <si>
+    <t>Marty</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Tooty</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Back End</t>
+  </si>
+  <si>
+    <t>Architecture</t>
   </si>
 </sst>
 </file>
@@ -435,19 +459,19 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.75" customWidth="1"/>
+    <col min="5" max="5" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -461,126 +485,127 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
         <v>7</v>
       </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
         <v>7</v>
       </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
         <v>7</v>
       </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
         <v>7</v>
       </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed Jayasree's update method
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>ProjectName</t>
   </si>
@@ -35,9 +35,6 @@
     <t>VerticalID</t>
   </si>
   <si>
-    <t>Excel Security</t>
-  </si>
-  <si>
     <t>Laura's Test Environment</t>
   </si>
   <si>
@@ -105,6 +102,18 @@
   </si>
   <si>
     <t>Architecture</t>
+  </si>
+  <si>
+    <t>Excel Security2</t>
+  </si>
+  <si>
+    <t>Excel Security3</t>
+  </si>
+  <si>
+    <t>Excel Security4</t>
+  </si>
+  <si>
+    <t>Excel Security5</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,123 +494,123 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>-1</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisions to ProjectUpdate/Update & ExcelDemo
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>ProjectName</t>
   </si>
@@ -104,16 +104,13 @@
     <t>Architecture</t>
   </si>
   <si>
-    <t>Excel Security2</t>
-  </si>
-  <si>
-    <t>Excel Security3</t>
-  </si>
-  <si>
-    <t>Excel Security4</t>
-  </si>
-  <si>
-    <t>Excel Security5</t>
+    <t>May 23 Project</t>
+  </si>
+  <si>
+    <t>Tomorrow's Project</t>
+  </si>
+  <si>
+    <t>Yesterday's Project</t>
   </si>
 </sst>
 </file>
@@ -468,7 +465,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +586,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>

<commit_message>
Sooo many, many changes...
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>ProjectName</t>
   </si>
@@ -104,13 +105,16 @@
     <t>Architecture</t>
   </si>
   <si>
-    <t>May 23 Project</t>
-  </si>
-  <si>
-    <t>Tomorrow's Project</t>
-  </si>
-  <si>
-    <t>Yesterday's Project</t>
+    <t>Online Test2</t>
+  </si>
+  <si>
+    <t>OnlineTest 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Test </t>
+  </si>
+  <si>
+    <t>Tuesday 24th</t>
   </si>
 </sst>
 </file>
@@ -462,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +512,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -530,88 +534,103 @@
       </c>
       <c r="H2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>-1</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added null check to GetAllProjectsForVertical
</commit_message>
<xml_diff>
--- a/ExcelDemo/JsonDemo.xlsx
+++ b/ExcelDemo/JsonDemo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>ProjectName</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Author</t>
   </si>
   <si>
-    <t>Add detail page</t>
-  </si>
-  <si>
     <t>Convert to UpdatePackage</t>
   </si>
   <si>
@@ -114,7 +111,16 @@
     <t xml:space="preserve">Online Test </t>
   </si>
   <si>
-    <t>Tuesday 24th</t>
+    <t>Saturday Works</t>
+  </si>
+  <si>
+    <t>Bits 10</t>
+  </si>
+  <si>
+    <t>New Landing page</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +518,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -521,19 +527,19 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +560,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1">
         <v>-1</v>
@@ -566,21 +572,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -592,21 +598,21 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -618,16 +624,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>